<commit_message>
done generate all possible route
</commit_message>
<xml_diff>
--- a/data_small2.xlsx
+++ b/data_small2.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FIP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Parameters</t>
   </si>
@@ -106,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="h\.mm;@"/>
+    <numFmt numFmtId="164" formatCode="h\.mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -206,25 +201,25 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -288,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -323,7 +318,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,7 +495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -510,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,8 +516,8 @@
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -543,7 +538,7 @@
         <v>35000</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="8">
@@ -552,7 +547,7 @@
       <c r="G2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -574,7 +569,7 @@
       <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -594,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="G4"/>
-      <c r="I4" s="16"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -609,11 +604,11 @@
       </c>
       <c r="E5" s="8">
         <f>COUNTIF(A9:A1048576,"Freight")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5" s="16"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G6"/>
@@ -623,221 +618,247 @@
       <c r="A7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="18"/>
+      <c r="F7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11" t="s">
+      <c r="F8" s="17"/>
+      <c r="G8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>0</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="10">
         <v>0</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <v>0</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>10</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="10">
         <f>SQRT((D10-B10)^2+(E10-C10)^2)</f>
         <v>10</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>10</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <v>10</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <v>10</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <v>-20</v>
       </c>
-      <c r="F11" s="12">
-        <f t="shared" ref="F11:F15" si="0">SQRT((D11-B11)^2+(E11-C11)^2)</f>
+      <c r="F11" s="10">
+        <f t="shared" ref="F11:F17" si="0">SQRT((D11-B11)^2+(E11-C11)^2)</f>
         <v>30</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>-5</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="10">
         <v>5</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="10">
         <v>15</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <v>0</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <f t="shared" si="0"/>
         <v>20.615528128088304</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <v>-10</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="10">
         <v>-10</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="10">
         <v>-10</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="10">
         <v>-20</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="10">
         <v>-6</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="10">
         <v>-6</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="10">
         <v>18</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="10">
         <v>3</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="10">
         <f t="shared" si="0"/>
         <v>25.632011235952593</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="A16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="10">
+        <v>-6</v>
+      </c>
+      <c r="C16" s="10">
+        <v>-15</v>
+      </c>
+      <c r="D16" s="10">
+        <v>-8</v>
+      </c>
+      <c r="E16" s="10">
+        <v>-20</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="0"/>
+        <v>5.3851648071345037</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="A17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="10">
+        <v>-5</v>
+      </c>
+      <c r="C17" s="10">
+        <v>6</v>
+      </c>
+      <c r="D17" s="10">
+        <v>5</v>
+      </c>
+      <c r="E17" s="10">
+        <v>12</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="0"/>
+        <v>11.661903789690601</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -850,102 +871,102 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>